<commit_message>
allow to refer with outer formula from parent to children
</commit_message>
<xml_diff>
--- a/core/modules/core/test/smoketest/crosstab.xlsx
+++ b/core/modules/core/test/smoketest/crosstab.xlsx
@@ -10,17 +10,17 @@
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Band1">data!$A$2</definedName>
-    <definedName name="Band2">data!$B$2</definedName>
-    <definedName name="DateHeader">data!$B$1</definedName>
-    <definedName name="Header">data!$A$1</definedName>
+    <definedName name="Band1">data!$A$2:$B$2</definedName>
+    <definedName name="Band2">data!$C$2</definedName>
+    <definedName name="DateHeader">data!$C$1</definedName>
+    <definedName name="Header">data!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>${income}</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -125,7 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -134,6 +137,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -436,34 +442,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="1" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4">
+        <f>SUM(C2:C2)</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>